<commit_message>
Formatted and cited BAPRiVMbVT
</commit_message>
<xml_diff>
--- a/InputData/trans/BAPRiVMbVT/BAU Annual Percent Reduction in Vehicle Mileage by Vehicle Type.xlsx
+++ b/InputData/trans/BAPRiVMbVT/BAU Annual Percent Reduction in Vehicle Mileage by Vehicle Type.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\BAPRiVMbVT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\BAPRiVMbVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{22788FC0-6F8A-45A6-AD42-44D06996DCAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269432E0-916C-4440-82D3-D8FE927757C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{BFAB966A-9411-4A1E-BACC-45FAF5B5983E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{BFAB966A-9411-4A1E-BACC-45FAF5B5983E}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <r>
       <rPr>
@@ -484,19 +484,46 @@
     <t>RMRs</t>
   </si>
   <si>
-    <t>Motorcycles using LDV for now, which is wrong</t>
-  </si>
-  <si>
     <t>miles/year</t>
-  </si>
-  <si>
-    <t>BAPRiVMbVT BAU Annual Reduction in Vehicle Milesage by Vehicle Type</t>
   </si>
   <si>
     <t>passenger</t>
   </si>
   <si>
     <t>freight</t>
+  </si>
+  <si>
+    <t>Sources:</t>
+  </si>
+  <si>
+    <t>Annual Vehicle Miles and Sales</t>
+  </si>
+  <si>
+    <t>Environmental Protection Agency</t>
+  </si>
+  <si>
+    <t>Population and Activity of Onroad Vehicles in MOVES3</t>
+  </si>
+  <si>
+    <t>https://pubs.acs.org/doi/pdf/10.1021/es505617p</t>
+  </si>
+  <si>
+    <t>Tables 6-1, 6-2, 6-3, and 4-4</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>This variable estimates the percentage annual reduction in VMT per vehicle.</t>
+  </si>
+  <si>
+    <t>We assume no reduction for non-road vehicles. Passenger motorbikes uses the value</t>
+  </si>
+  <si>
+    <t>for passenger LDVs</t>
+  </si>
+  <si>
+    <t>BAPRiVMbVT BAU Annual Reduction in Vehicle Mileage by Vehicle Type</t>
   </si>
 </sst>
 </file>
@@ -511,13 +538,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -566,6 +586,14 @@
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -576,12 +604,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -708,101 +737,110 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5064,23 +5102,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BCDA94-FCB9-42AB-AE4A-6D13A2EF093A}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="66.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>49</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="34">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{D8AE217F-17B2-47B2-A63C-BB97D3FFDFA7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5089,8 +5181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D25A5B-E3B7-4852-A6C5-2A76687F0867}">
   <dimension ref="A1:AN90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J36" sqref="A34:J36"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H33" sqref="A33:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5100,10 +5192,10 @@
   <sheetData>
     <row r="1" spans="1:40" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25"/>
+      <c r="C1" s="24"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3" t="s">
         <v>1</v>
@@ -5215,7 +5307,7 @@
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="23" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -5314,7 +5406,7 @@
       <c r="C3" s="5">
         <v>15806</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
@@ -6169,25 +6261,25 @@
       <c r="G70" s="8"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="26" t="s">
+      <c r="A71" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B71" s="28" t="s">
+      <c r="B71" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C71" s="30" t="s">
+      <c r="C71" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D71" s="31"/>
-      <c r="E71" s="32"/>
-      <c r="F71" s="30" t="s">
+      <c r="D71" s="30"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="G71" s="32"/>
+      <c r="G71" s="31"/>
     </row>
     <row r="72" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="27"/>
-      <c r="B72" s="29"/>
+      <c r="A72" s="26"/>
+      <c r="B72" s="28"/>
       <c r="C72" s="3" t="s">
         <v>41</v>
       </c>
@@ -6635,8 +6727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD2172E-F1BF-496B-B095-8A637E660678}">
   <dimension ref="A1:X40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K29" sqref="A28:K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8760,7 +8852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4923C903-F0FF-4839-859F-48877529C182}">
   <dimension ref="A1:AF12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
@@ -9771,7 +9863,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -9782,13 +9874,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -9817,7 +9909,7 @@
       <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="22">
         <v>0</v>
       </c>
       <c r="C4">
@@ -9828,7 +9920,7 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="22">
         <v>0</v>
       </c>
       <c r="C5">
@@ -9839,7 +9931,7 @@
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>0</v>
       </c>
       <c r="C6">

</xml_diff>